<commit_message>
all output fields to be used in the combo_order_eval table must have values
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/combo_order_eval.xlsx
+++ b/rufus/carriers/lifemap_science/order/combo_order_eval.xlsx
@@ -54,18 +54,12 @@
     <t>${ProSpec price}</t>
   </si>
   <si>
-    <t>${r:${BioTime price} + ${ProSpec price}}</t>
-  </si>
-  <si>
     <t>${BioTime Handling}</t>
   </si>
   <si>
     <t>${ProSpec Handling}</t>
   </si>
   <si>
-    <t>${r:${BioTime Handling} + ${ProSpec Handling}}</t>
-  </si>
-  <si>
     <t>$in = $(BioTime, ProSpec)</t>
   </si>
   <si>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>${r:'${BioTime Shipping Method}' + ', ' +' ${ProSpec Shipping Method}'}</t>
+  </si>
+  <si>
+    <t>${r:${BioTime price}.to_i + ${ProSpec price}.to_i}</t>
+  </si>
+  <si>
+    <t>${r:${BioTime Handling}.to_i + ${ProSpec Handling}.to_i}</t>
   </si>
 </sst>
 </file>
@@ -712,7 +712,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -720,7 +720,7 @@
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="57.5" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -753,13 +753,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -771,14 +771,14 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>10</v>
@@ -793,19 +793,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>

</xml_diff>